<commit_message>
Redid analysis for apartments
</commit_message>
<xml_diff>
--- a/Results-Graphs/Kruskal_AllData.xlsx
+++ b/Results-Graphs/Kruskal_AllData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,16 +458,70 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Building_state_regroup</t>
+          <t>Locality</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>491.4437616404966</v>
+        <v>3387.042544212517</v>
       </c>
       <c r="C2" t="n">
-        <v>3.411152075556571e-106</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
+        <is>
+          <t>Significant</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Type of property</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>230.8120164564934</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.96512301509665e-52</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Significant</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Subtype of property</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1275.10090185504</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5.133558478747024e-257</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Significant</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>State of the building</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>572.6279869382911</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.86681536684807e-120</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>Significant</t>
         </is>

</xml_diff>